<commit_message>
final updates about cost page-1
</commit_message>
<xml_diff>
--- a/src/test/resources/Vytracktestdata.xlsx
+++ b/src/test/resources/Vytracktestdata.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3763" uniqueCount="1475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3765" uniqueCount="1475">
   <si>
     <t>username</t>
   </si>
@@ -4798,7 +4798,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -13588,10 +13588,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="223" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13613,6 +13613,14 @@
         <v>133</v>
       </c>
       <c r="B2" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" t="s">
         <v>1472</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some new change about test hw
</commit_message>
<xml_diff>
--- a/src/test/resources/Vytracktestdata.xlsx
+++ b/src/test/resources/Vytracktestdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="33600" windowHeight="16416" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="33600" windowHeight="16416" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="QA1-all" sheetId="4" r:id="rId1"/>
@@ -13,6 +13,8 @@
     <sheet name="QA2-short" sheetId="3" r:id="rId4"/>
     <sheet name="QA3-all" sheetId="1" r:id="rId5"/>
     <sheet name="QA3-short" sheetId="7" r:id="rId6"/>
+    <sheet name="HW" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3765" uniqueCount="1475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3787" uniqueCount="1492">
   <si>
     <t>username</t>
   </si>
@@ -4455,15 +4457,73 @@
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>All-Day Event</t>
+  </si>
+  <si>
+    <t>Organizer</t>
+  </si>
+  <si>
+    <t>Guests</t>
+  </si>
+  <si>
+    <t>Recurrence</t>
+  </si>
+  <si>
+    <t>Call Via Hangout</t>
+  </si>
+  <si>
+    <t>This is a a weekly testers meeting</t>
+  </si>
+  <si>
+    <t>Testers meeting</t>
+  </si>
+  <si>
+    <t>Nov 27, 2019, 9:30 AM</t>
+  </si>
+  <si>
+    <t>Nov 27, 2019, 10:30 AM</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Stephan Haley</t>
+  </si>
+  <si>
+    <t>Tom Smith</t>
+  </si>
+  <si>
+    <t>Weekly every 1 week on Wednesday</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -4490,8 +4550,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4798,7 +4859,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -13590,8 +13651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="223" workbookViewId="0">
-      <selection activeCell="B6" sqref="B5:B6"/>
+    <sheetView zoomScale="223" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -18090,4 +18151,131 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>